<commit_message>
updated ori synth landmarks
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_evaluation/landmark_points_full.xlsx
+++ b/franz_hsa/landmark_evaluation/landmark_points_full.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C3511D-DFF2-469E-99C3-8D8AC7C7E0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9397AA6-D90E-43B2-8D02-C312D6ECED19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11196" yWindow="12912" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -457,7 +457,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +502,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>138</v>
+        <v>10278</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -510,7 +510,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>5752</v>
+        <v>8793</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -558,7 +558,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>8232</v>
+        <v>5335</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>